<commit_message>
Updated analysis data and stored logs that go into thesis in a separate folder
</commit_message>
<xml_diff>
--- a/analysis/Labelled design vs Range queries Benchmark.xlsx
+++ b/analysis/Labelled design vs Range queries Benchmark.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,12 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="18960" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="44460" windowHeight="21660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Last" sheetId="2" r:id="rId1"/>
+    <sheet name="First Attempt" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Last!$L$21:$L$23</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Last!$M$20</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Last!$M$21:$M$23</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Last!$N$20</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Last!$N$21:$N$23</definedName>
+  </definedNames>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="24">
   <si>
     <t>[1000]</t>
   </si>
@@ -61,11 +69,50 @@
   <si>
     <t>Labelled</t>
   </si>
+  <si>
+    <t>CHUNKED</t>
+  </si>
+  <si>
+    <t>Labelled Design</t>
+  </si>
+  <si>
+    <t>Range Retrieval Times</t>
+  </si>
+  <si>
+    <t>СHUNKED &amp; COMPRESSED</t>
+  </si>
+  <si>
+    <t>Range Retrieval</t>
+  </si>
+  <si>
+    <t>СHUNKED, COMPRESSED, ENCRYPTED</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>1st repetition</t>
+  </si>
+  <si>
+    <t>2nd repetition</t>
+  </si>
+  <si>
+    <t>3rd repetition</t>
+  </si>
+  <si>
+    <t>Low Temperature Range</t>
+  </si>
+  <si>
+    <t>Middle Temperature Range</t>
+  </si>
+  <si>
+    <t>High Temperature Range</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -149,7 +196,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -158,6 +205,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -169,12 +217,612 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Retrieval</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Times for Chunked, Compressed and Encrypted </a:t>
+            </a:r>
+            <a:endParaRPr lang="ru-RU" baseline="0"/>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>Ava Entries in HyperDex</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Last!$M$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Range Retrieval</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inBase"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Last!$L$21:$L$23</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Low Temperature Range</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Middle Temperature Range</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>High Temperature Range</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Last!$M$21:$M$23</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>68.272868333333335</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>126.81982633333332</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>155.41926900000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-59D6-C548-BFD6-E7946E11C026}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Last!$N$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Labelled Design</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Last!$L$21:$L$23</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Low Temperature Range</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Middle Temperature Range</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>High Temperature Range</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Last!$N$21:$N$23</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>9.4882666666666671E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.11227166666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.875266666666666E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-59D6-C548-BFD6-E7946E11C026}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="349042144"/>
+        <c:axId val="375402976"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="349042144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="375402976"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="375402976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>	</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>, ms</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="349042144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -234,7 +882,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -276,7 +923,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$25</c:f>
+              <c:f>'First Attempt'!$C$25</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -297,7 +944,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$26:$B$29</c:f>
+              <c:f>'First Attempt'!$B$26:$B$29</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -317,32 +964,37 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$26:$C$29</c:f>
+              <c:f>'First Attempt'!$C$26:$C$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.306967666666667</c:v>
+                  <c:v>0.30696766666666669</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>85.52352633333334</c:v>
+                  <c:v>85.523526333333336</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>107.5240233333333</c:v>
+                  <c:v>107.52402333333333</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>149.2179323333333</c:v>
+                  <c:v>149.21793233333332</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-231A-4843-8FA2-2CB26C100456}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$25</c:f>
+              <c:f>'First Attempt'!$D$25</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -363,7 +1015,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$26:$B$29</c:f>
+              <c:f>'First Attempt'!$B$26:$B$29</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -383,32 +1035,37 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$26:$D$29</c:f>
+              <c:f>'First Attempt'!$D$26:$D$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.0997383333333333</c:v>
+                  <c:v>9.9738333333333332E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60.418231</c:v>
+                  <c:v>60.418230999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>101.7626693333333</c:v>
+                  <c:v>101.76266933333333</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>144.9257946666667</c:v>
+                  <c:v>144.92579466666666</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-231A-4843-8FA2-2CB26C100456}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$25</c:f>
+              <c:f>'First Attempt'!$E$25</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -429,7 +1086,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$26:$B$29</c:f>
+              <c:f>'First Attempt'!$B$26:$B$29</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -449,25 +1106,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$26:$E$29</c:f>
+              <c:f>'First Attempt'!$E$26:$E$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.0990566666666666</c:v>
+                  <c:v>9.9056666666666668E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60.25847033333333</c:v>
+                  <c:v>60.258470333333328</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>110.4676836666667</c:v>
+                  <c:v>110.46768366666667</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>148.1244536666667</c:v>
+                  <c:v>148.12445366666665</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-231A-4843-8FA2-2CB26C100456}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -580,7 +1242,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -610,6 +1271,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -654,7 +1316,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -761,6 +1422,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -1264,7 +1965,551 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>658091</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>53542</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>728806</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>170151</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6B5095B-CD6F-1340-A09C-C530B51A8C9C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1281,7 +2526,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1561,10 +2812,482 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E07183A8-74AD-F840-A3B4-E294D33A8763}">
+  <dimension ref="A1:N27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="176" workbookViewId="0">
+      <selection activeCell="O27" sqref="O27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0.38627</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>0.30626500000000001</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>0.33749699999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>0.36567300000000003</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>0.29993599999999998</v>
+      </c>
+      <c r="H4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>0.32249499999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>0.34372799999999998</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>0.39765099999999998</v>
+      </c>
+      <c r="H5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>0.30778499999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>62.383074999999998</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>58.072938000000001</v>
+      </c>
+      <c r="H7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>61.793883000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>112.62817099999999</v>
+      </c>
+      <c r="E8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>105.13851699999999</v>
+      </c>
+      <c r="H8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8">
+        <v>122.75962699999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>153.62005099999999</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>155.72800000000001</v>
+      </c>
+      <c r="H9" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9">
+        <v>169.53420800000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>0.103834</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0.15821199999999999</v>
+      </c>
+      <c r="H12" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>0.10723299999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>9.4909999999999994E-2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>9.8822999999999994E-2</v>
+      </c>
+      <c r="H13" t="s">
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <v>8.7970999999999994E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>9.1691999999999996E-2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <v>0.106893</v>
+      </c>
+      <c r="H14" t="s">
+        <v>3</v>
+      </c>
+      <c r="I14">
+        <v>8.405E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>60.955545000000001</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>111.553597</v>
+      </c>
+      <c r="H16" t="s">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>65.373705999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>104.107592</v>
+      </c>
+      <c r="E17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>148.690979</v>
+      </c>
+      <c r="H17" t="s">
+        <v>2</v>
+      </c>
+      <c r="I17">
+        <v>114.307256</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>148.95963900000001</v>
+      </c>
+      <c r="E18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18">
+        <v>161.61112199999999</v>
+      </c>
+      <c r="H18" t="s">
+        <v>3</v>
+      </c>
+      <c r="I18">
+        <v>150.50401299999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M20" t="s">
+        <v>15</v>
+      </c>
+      <c r="N20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>9.7393999999999994E-2</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>9.3672000000000005E-2</v>
+      </c>
+      <c r="H21" t="s">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>9.3581999999999999E-2</v>
+      </c>
+      <c r="L21" t="s">
+        <v>21</v>
+      </c>
+      <c r="M21" s="6">
+        <f>AVERAGE(C25,F25,I25)</f>
+        <v>68.272868333333335</v>
+      </c>
+      <c r="N21" s="6">
+        <f>AVERAGE(C21,F21,I21)</f>
+        <v>9.4882666666666671E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>0.126138</v>
+      </c>
+      <c r="E22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22">
+        <v>8.9101E-2</v>
+      </c>
+      <c r="H22" t="s">
+        <v>2</v>
+      </c>
+      <c r="I22">
+        <v>0.121576</v>
+      </c>
+      <c r="L22" t="s">
+        <v>22</v>
+      </c>
+      <c r="M22" s="6">
+        <f>AVERAGE(C26,F26,I26)</f>
+        <v>126.81982633333332</v>
+      </c>
+      <c r="N22" s="6">
+        <f t="shared" ref="N22:N23" si="0">AVERAGE(C22,F22,I22)</f>
+        <v>0.11227166666666667</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23">
+        <v>8.9690000000000006E-2</v>
+      </c>
+      <c r="E23" t="s">
+        <v>3</v>
+      </c>
+      <c r="F23">
+        <v>9.0942999999999996E-2</v>
+      </c>
+      <c r="H23" t="s">
+        <v>3</v>
+      </c>
+      <c r="I23">
+        <v>8.5625000000000007E-2</v>
+      </c>
+      <c r="L23" t="s">
+        <v>23</v>
+      </c>
+      <c r="M23" s="6">
+        <f>AVERAGE(C27,F27,I27)</f>
+        <v>155.41926900000001</v>
+      </c>
+      <c r="N23" s="6">
+        <f>AVERAGE(C23,F23,I23)</f>
+        <v>8.875266666666666E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>81.817301999999998</v>
+      </c>
+      <c r="E25" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>62.963397999999998</v>
+      </c>
+      <c r="H25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>60.037905000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>151.20978500000001</v>
+      </c>
+      <c r="E26" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26">
+        <v>124.423839</v>
+      </c>
+      <c r="H26" t="s">
+        <v>2</v>
+      </c>
+      <c r="I26">
+        <v>104.825855</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <v>158.47659300000001</v>
+      </c>
+      <c r="E27" t="s">
+        <v>3</v>
+      </c>
+      <c r="F27">
+        <v>162.359847</v>
+      </c>
+      <c r="H27" t="s">
+        <v>3</v>
+      </c>
+      <c r="I27">
+        <v>145.421367</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A13" zoomScale="163" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="A4" zoomScale="163" workbookViewId="0">
       <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
@@ -2049,7 +3772,7 @@
         <v>149.21793233333332</v>
       </c>
       <c r="D29">
-        <f t="shared" ref="D27:D29" si="5">G21</f>
+        <f t="shared" ref="D29" si="5">G21</f>
         <v>144.92579466666666</v>
       </c>
       <c r="E29">

</xml_diff>